<commit_message>
Added cascade optimization examples
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_sir.xlsx
+++ b/tests/databooks/progbook_sir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1461CF-63B2-4EF6-B89E-A1110E4CABBF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26309013-4B31-4E04-AF06-CC7E63B0708F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="255" yWindow="765" windowWidth="24945" windowHeight="13395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1401,7 +1401,7 @@
   <dimension ref="B1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>